<commit_message>
fixed excel sheet, web scraping code works
put the item name, and total in first column to allow the web tool to overwrite without messing the other rows.
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11994CC0-4D49-445E-9C72-357BB9167A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2082AC27-0C11-4C3C-A066-D21DB11C1F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="683" yWindow="3128" windowWidth="14399" windowHeight="8272" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>First Name</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>ItemName</t>
-  </si>
-  <si>
-    <t>CustomerID</t>
   </si>
 </sst>
 </file>
@@ -442,96 +439,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23614267-4752-4D6C-B353-C7D81967B51D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>2</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>3</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>4</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>5</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
prints out dirty data of price version
price feature done
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2082AC27-0C11-4C3C-A066-D21DB11C1F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942FBFD9-2809-4DCA-B7AE-94AFBE5E1749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="683" yWindow="3128" windowWidth="14399" windowHeight="8272" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="3690" yWindow="1500" windowWidth="14400" windowHeight="8273" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>First Name</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Jeans</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
   <si>
     <t>ItemName</t>
@@ -439,77 +442,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23614267-4752-4D6C-B353-C7D81967B51D}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clean print out of the price version
price is printing without extra characters.
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942FBFD9-2809-4DCA-B7AE-94AFBE5E1749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26994AF-63B0-40D3-B5F8-0380910C3B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="1500" windowWidth="14400" windowHeight="8273" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="3893" yWindow="997" windowWidth="14400" windowHeight="8273" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -54,43 +48,46 @@
     <t>Smith</t>
   </si>
   <si>
+    <t>Haskel</t>
+  </si>
+  <si>
+    <t>Lott</t>
+  </si>
+  <si>
+    <t>Mikey</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Burger</t>
+  </si>
+  <si>
+    <t>Flowers</t>
+  </si>
+  <si>
+    <t>Jeans</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>ItemName</t>
+  </si>
+  <si>
     <t>Tasha</t>
   </si>
   <si>
     <t>Locke</t>
   </si>
   <si>
-    <t>Haskel</t>
-  </si>
-  <si>
-    <t>Lott</t>
-  </si>
-  <si>
-    <t>Mikey</t>
-  </si>
-  <si>
-    <t>Mouse</t>
-  </si>
-  <si>
-    <t>Burger</t>
-  </si>
-  <si>
     <t>Car</t>
   </si>
   <si>
-    <t>iphone</t>
-  </si>
-  <si>
-    <t>Flowers</t>
-  </si>
-  <si>
-    <t>Jeans</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>ItemName</t>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
   </si>
 </sst>
 </file>
@@ -445,78 +442,78 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creates sheet2 and save the output in there
create a new sheet within the same excel file to save data.
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26994AF-63B0-40D3-B5F8-0380910C3B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8C9F545-314B-4551-BE00-E06FE0EBAEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3893" yWindow="997" windowWidth="14400" windowHeight="8273" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="0" yWindow="3128" windowWidth="14400" windowHeight="8272" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Jeans</t>
-  </si>
-  <si>
-    <t>Price</t>
   </si>
   <si>
     <t>ItemName</t>
@@ -439,80 +436,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23614267-4752-4D6C-B353-C7D81967B51D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
       <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
all constrains and 3 MVP are met
constrains and most MVP are met
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26994AF-63B0-40D3-B5F8-0380910C3B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53FB011-536E-4A10-AFB2-4B8CB1CFD51E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3893" yWindow="997" windowWidth="14400" windowHeight="8273" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="698" yWindow="3098" windowWidth="14400" windowHeight="8272" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -69,9 +69,6 @@
     <t>Jeans</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>ItemName</t>
   </si>
   <si>
@@ -88,6 +85,24 @@
   </si>
   <si>
     <t>LastName</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>Baraka</t>
+  </si>
+  <si>
+    <t>Jet</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Alfaro</t>
   </si>
 </sst>
 </file>
@@ -439,81 +454,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23614267-4752-4D6C-B353-C7D81967B51D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
       <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added PlaceOrder xaml and edited excel sheets
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donation\Desktop\Baraka_H-andAlfaro_G-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF1F0D0-D66E-4259-9F99-7260DBE8DFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A7020B-4104-4C09-917E-97593C936312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="698" yWindow="3098" windowWidth="14400" windowHeight="8272" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="9795" yWindow="2970" windowWidth="14565" windowHeight="8310" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -54,9 +54,6 @@
     <t>Flowers</t>
   </si>
   <si>
-    <t>ItemName</t>
-  </si>
-  <si>
     <t>Tasha</t>
   </si>
   <si>
@@ -79,6 +76,36 @@
   </si>
   <si>
     <t>Baraka</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Item1</t>
+  </si>
+  <si>
+    <t>Qty1</t>
+  </si>
+  <si>
+    <t>Item2</t>
+  </si>
+  <si>
+    <t>Qty2</t>
+  </si>
+  <si>
+    <t>Item3</t>
+  </si>
+  <si>
+    <t>Qty3</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Walmart</t>
   </si>
 </sst>
 </file>
@@ -430,28 +457,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23614267-4752-4D6C-B353-C7D81967B51D}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -459,10 +504,16 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -470,27 +521,45 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+      <c r="E4">
+        <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
discount feature added in excell sheet
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFBB6A8-5355-4DF8-9363-0CA509058E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC5B16E-FF2C-459C-A8A7-B79587DF2C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="698" yWindow="3098" windowWidth="14400" windowHeight="8272" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="3000" yWindow="5168" windowWidth="14400" windowHeight="6045" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -72,30 +72,15 @@
     <t>Watch</t>
   </si>
   <si>
-    <t>Hassan</t>
-  </si>
-  <si>
-    <t>Baraka</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
-    <t>Item1</t>
-  </si>
-  <si>
     <t>Qty1</t>
   </si>
   <si>
-    <t>Item2</t>
-  </si>
-  <si>
     <t>Qty2</t>
   </si>
   <si>
-    <t>Item3</t>
-  </si>
-  <si>
     <t>Qty3</t>
   </si>
   <si>
@@ -105,16 +90,25 @@
     <t>Target</t>
   </si>
   <si>
-    <t>Walmart</t>
-  </si>
-  <si>
-    <t>Book</t>
-  </si>
-  <si>
-    <t>Gabriel</t>
-  </si>
-  <si>
-    <t>Alfaro</t>
+    <t>ItemName</t>
+  </si>
+  <si>
+    <t>ItemName2</t>
+  </si>
+  <si>
+    <t>ItemName3</t>
+  </si>
+  <si>
+    <t>Uber eats</t>
+  </si>
+  <si>
+    <t>Carvana</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>James</t>
   </si>
 </sst>
 </file>
@@ -466,17 +460,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23614267-4752-4D6C-B353-C7D81967B51D}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.06640625" customWidth="1"/>
+    <col min="5" max="5" width="11.9296875" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -485,27 +484,27 @@
         <v>10</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -513,16 +512,16 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2">
+      <c r="D2">
         <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -530,16 +529,16 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -547,39 +546,28 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
         <v>5</v>
       </c>
-      <c r="E4">
-        <v>5</v>
+      <c r="I4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
+        <v>24</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
+      <c r="I5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Email shoppers and vendors feature is added
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC5B16E-FF2C-459C-A8A7-B79587DF2C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C162A2-28F5-44D9-927E-784CF4F14475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="5168" windowWidth="14400" windowHeight="6045" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="1972" yWindow="4403" windowWidth="14401" windowHeight="6045" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>James</t>
+  </si>
+  <si>
+    <t>T-shirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hassan </t>
+  </si>
+  <si>
+    <t>Baraka</t>
   </si>
 </sst>
 </file>
@@ -460,7 +469,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23614267-4752-4D6C-B353-C7D81967B51D}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -570,6 +579,17 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made skeleton for Adding Expense and Formatted Excel Sheets
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donation\Desktop\Baraka_H-andAlfaro_G-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFBB6A8-5355-4DF8-9363-0CA509058E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1434AC6-6DE9-4340-AB7E-12A5EDD4BEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="698" yWindow="3098" windowWidth="14400" windowHeight="8272" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="-17445" yWindow="2430" windowWidth="14565" windowHeight="8310" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -108,13 +108,13 @@
     <t>Walmart</t>
   </si>
   <si>
-    <t>Book</t>
-  </si>
-  <si>
     <t>Gabriel</t>
   </si>
   <si>
     <t>Alfaro</t>
+  </si>
+  <si>
+    <t>Towel</t>
   </si>
 </sst>
 </file>
@@ -469,12 +469,12 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -503,7 +503,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -520,7 +520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -537,7 +537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -554,7 +554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -571,15 +571,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>26</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Place order without UI
place order sequence separated from add client. Also expanse and client sheets were modified.
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C162A2-28F5-44D9-927E-784CF4F14475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC07C73-035C-4413-8FC7-D2189BEB7641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1972" yWindow="4403" windowWidth="14401" windowHeight="6045" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="2370" yWindow="4545" windowWidth="14400" windowHeight="6045" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -111,23 +111,64 @@
     <t>James</t>
   </si>
   <si>
-    <t>T-shirt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hassan </t>
-  </si>
-  <si>
-    <t>Baraka</t>
+    <t>CustomerEmail</t>
+  </si>
+  <si>
+    <t>VendorEmail</t>
+  </si>
+  <si>
+    <t>johnDoe@outlook.com</t>
+  </si>
+  <si>
+    <t>marysmith@outlook.com</t>
+  </si>
+  <si>
+    <t>tLocke@gmail.com</t>
+  </si>
+  <si>
+    <t>OliviaJ@Yahoo.com</t>
+  </si>
+  <si>
+    <t>ubereats@outllok.com</t>
+  </si>
+  <si>
+    <t>carvanacars@outlook.com</t>
+  </si>
+  <si>
+    <t>targetshooper@gmail.com</t>
+  </si>
+  <si>
+    <t>amazonbuy@gmail.com</t>
+  </si>
+  <si>
+    <t>Belt</t>
+  </si>
+  <si>
+    <t>Baby Yoda</t>
+  </si>
+  <si>
+    <t>Jeans</t>
+  </si>
+  <si>
+    <t>OrderNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,13 +191,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -469,128 +513,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23614267-4752-4D6C-B353-C7D81967B51D}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" customWidth="1"/>
-    <col min="5" max="5" width="11.9296875" customWidth="1"/>
-    <col min="7" max="7" width="11.3984375" customWidth="1"/>
+    <col min="1" max="1" width="12.19921875" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" customWidth="1"/>
+    <col min="6" max="6" width="11.9296875" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
+    <col min="13" max="13" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
         <v>17</v>
       </c>
+      <c r="K4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="I5" t="s">
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{5213C1F4-591E-49F6-8AF5-C82F1067F363}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{E307C78A-3F20-41C1-9F34-AD80508908F4}"/>
+    <hyperlink ref="K4" r:id="rId3" xr:uid="{242BE019-F871-4765-BBBE-8B810B97D039}"/>
+    <hyperlink ref="K5" r:id="rId4" xr:uid="{C6A0C15B-5B82-41A5-AA48-59C5479D2B8C}"/>
+    <hyperlink ref="L2" r:id="rId5" xr:uid="{3F0ACC9A-810B-4699-8B85-E00F51A82967}"/>
+    <hyperlink ref="L3" r:id="rId6" xr:uid="{38D4F16E-3377-4539-9640-D0FF42850DE7}"/>
+    <hyperlink ref="L4" r:id="rId7" xr:uid="{A350A06D-83BF-4EB2-B257-83EA98292B58}"/>
+    <hyperlink ref="L5" r:id="rId8" xr:uid="{CA89A31A-86BA-4E62-A3FC-0C38612C9DF3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed addExpense and took out confusing code
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donation\Desktop\Baraka_H-andAlfaro_G-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1434AC6-6DE9-4340-AB7E-12A5EDD4BEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47499419-AE84-4653-8CB8-81C3CBD917A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17445" yWindow="2430" windowWidth="14565" windowHeight="8310" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="-17130" yWindow="2430" windowWidth="14565" windowHeight="8310" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -48,21 +48,12 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>Burger</t>
-  </si>
-  <si>
-    <t>Flowers</t>
-  </si>
-  <si>
     <t>Tasha</t>
   </si>
   <si>
     <t>Locke</t>
   </si>
   <si>
-    <t>Car</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -115,6 +106,27 @@
   </si>
   <si>
     <t>Towel</t>
+  </si>
+  <si>
+    <t>Bike</t>
+  </si>
+  <si>
+    <t>Baseball</t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>Candy</t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t>Camera</t>
   </si>
 </sst>
 </file>
@@ -469,43 +481,51 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -514,15 +534,27 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -531,61 +563,109 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
         <v>26</v>
       </c>
       <c r="E6">
         <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
email attachment edits, added demo video
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0515FA-7F6E-4AE8-91E3-8AFC3451504E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E46C15E-65B8-477C-A7A6-377D9F68AA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="4665" windowWidth="14242" windowHeight="6045" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="1530" yWindow="5355" windowWidth="14400" windowHeight="6045" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
made expense sheet1 work
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donation\Desktop\Baraka_H-andAlfaro_G-P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47499419-AE84-4653-8CB8-81C3CBD917A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA8B0E5-F37F-4882-B990-8D0ED39945CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17130" yWindow="2430" windowWidth="14565" windowHeight="8310" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="-16965" yWindow="2760" windowWidth="14565" windowHeight="8310" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -96,9 +96,6 @@
     <t>Target</t>
   </si>
   <si>
-    <t>Walmart</t>
-  </si>
-  <si>
     <t>Gabriel</t>
   </si>
   <si>
@@ -111,15 +108,6 @@
     <t>Bike</t>
   </si>
   <si>
-    <t>Baseball</t>
-  </si>
-  <si>
-    <t>Shirt</t>
-  </si>
-  <si>
-    <t>Pants</t>
-  </si>
-  <si>
     <t>Candy</t>
   </si>
   <si>
@@ -127,6 +115,30 @@
   </si>
   <si>
     <t>Camera</t>
+  </si>
+  <si>
+    <t>Uber Eats</t>
+  </si>
+  <si>
+    <t>Burger</t>
+  </si>
+  <si>
+    <t>Red Wine</t>
+  </si>
+  <si>
+    <t>Beef Steak</t>
+  </si>
+  <si>
+    <t>Carvana</t>
+  </si>
+  <si>
+    <t>Truck</t>
+  </si>
+  <si>
+    <t>SUV</t>
+  </si>
+  <si>
+    <t>Car</t>
   </si>
 </sst>
 </file>
@@ -481,7 +493,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,13 +552,13 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -554,7 +566,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -563,19 +575,19 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -592,19 +604,19 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G4">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -627,13 +639,13 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5">
         <v>3</v>
@@ -641,31 +653,31 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nothing new just deleted the data created when we run the code in demo.
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donation\Desktop\Baraka_H-andAlfaro_G-P0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\hbksilver-code\RPA\P0\P0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F560D7-B3C0-47FF-822F-891F1F22D082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5265EB1-E571-4D6E-BA14-F8C25371184A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7665" yWindow="3060" windowWidth="14565" windowHeight="8310" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
+    <workbookView xWindow="1567" yWindow="3075" windowWidth="14401" windowHeight="7672" xr2:uid="{E8966CE7-3C57-45EB-98D1-2A925D107EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">John </t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>Item</t>
+  </si>
+  <si>
+    <t>OrderNumber</t>
   </si>
 </sst>
 </file>
@@ -472,19 +475,22 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" customWidth="1"/>
+    <col min="11" max="11" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
       <c r="B1" t="s">
         <v>27</v>
       </c>
@@ -513,7 +519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -539,7 +545,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -565,7 +571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -594,7 +600,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>

</xml_diff>